<commit_message>
ng: add kebbi forms
</commit_message>
<xml_diff>
--- a/LF/TAS/Nigeria/2024/june_2024/Kebbi/ng_lf_tas_2406_2_fts_kb.xlsx
+++ b/LF/TAS/Nigeria/2024/june_2024/Kebbi/ng_lf_tas_2406_2_fts_kb.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bonhe\Repositories\dsa-forms\LF\TAS\Nigeria\2024\june_2024\Niger\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bonhe\Repositories\dsa-forms\LF\TAS\Nigeria\2024\june_2024\Kebbi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76691E9-E7F7-4ECD-9A3F-80D0A125D3BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C7C0DD-1B05-4711-A33F-210CDAE65D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -532,13 +532,13 @@
     <t>10</t>
   </si>
   <si>
-    <t>ng_lf_tas_2406_2_fts_ng</t>
-  </si>
-  <si>
-    <t>(June 2024) - 2. Niger - TAS1 LF FTS Form V2</t>
-  </si>
-  <si>
-    <t>ng_tas_fts_2406_ng</t>
+    <t>ng_tas_fts_2406_kb</t>
+  </si>
+  <si>
+    <t>(June 2024) - 2. Kabbi - TAS1 LF FTS Form</t>
+  </si>
+  <si>
+    <t>ng_lf_tas_2406_2_fts_kb</t>
   </si>
 </sst>
 </file>
@@ -1094,7 +1094,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -1336,7 +1336,7 @@
         <v>100</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>107</v>
@@ -3516,8 +3516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3547,7 +3547,7 @@
         <v>165</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C2" s="27" t="s">
         <v>97</v>

</xml_diff>